<commit_message>
Updated openAI with pandasai model and TAPAS with basic check
</commit_message>
<xml_diff>
--- a/sample_data/09 JULY 2023 DEWAS.xlsx
+++ b/sample_data/09 JULY 2023 DEWAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6790"/>
+    <workbookView windowWidth="18350" windowHeight="6830"/>
   </bookViews>
   <sheets>
     <sheet name="export - 2023-07-09T094213.092" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -696,9 +696,14 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,10 +1026,13 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="4" width="15.2727272727273" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -1036,7 +1044,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1068,7 +1076,7 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>44965.6876273148</v>
       </c>
       <c r="E2">
@@ -1101,7 +1109,7 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>44965.6876273148</v>
       </c>
       <c r="E3">
@@ -1134,7 +1142,7 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>44979.1877314815</v>
       </c>
       <c r="E4">
@@ -1167,7 +1175,7 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>45020.3544560185</v>
       </c>
       <c r="E5">
@@ -1200,7 +1208,7 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>45082.5213194444</v>
       </c>
       <c r="E6">
@@ -1233,7 +1241,7 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>45099.5212847222</v>
       </c>
       <c r="E7">
@@ -1266,7 +1274,7 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>45099.5212847222</v>
       </c>
       <c r="E8">
@@ -1299,7 +1307,7 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>45105.5210416667</v>
       </c>
       <c r="E9">
@@ -1332,7 +1340,7 @@
       <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>45105.5210416667</v>
       </c>
       <c r="E10">
@@ -1365,7 +1373,7 @@
       <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>45105.5210416667</v>
       </c>
       <c r="E11">
@@ -1398,7 +1406,7 @@
       <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>45105.5210416667</v>
       </c>
       <c r="E12">
@@ -1431,7 +1439,7 @@
       <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>45106.3547569444</v>
       </c>
       <c r="E13">
@@ -1464,7 +1472,7 @@
       <c r="C14" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>45112.3544097222</v>
       </c>
       <c r="E14">

</xml_diff>